<commit_message>
Actualizacion de Saul de funciones de Z_parameter
</commit_message>
<xml_diff>
--- a/Netlist.xlsx
+++ b/Netlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monts\OneDrive\Documentos\Escuela\Cinvestav\Primer Cuatrimestre\RFI\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0D7730-9DD6-43B3-9A87-2EBD4C05BFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA46FDD9-E678-4790-B81E-1B973E40D7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{123A8AA9-D291-44EE-A285-0562C51A2FBD}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,6 +542,12 @@
       <c r="E3" s="1">
         <v>53</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -559,6 +565,12 @@
       <c r="E4" s="4">
         <v>4.6999999999999997E-8</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -575,6 +587,12 @@
       </c>
       <c r="E5" s="1">
         <v>95</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
       </c>
       <c r="I5" s="3"/>
     </row>

</xml_diff>

<commit_message>
Funcion Sparameters para distribuidos, y fnciones no usadas eliminadas
</commit_message>
<xml_diff>
--- a/Netlist.xlsx
+++ b/Netlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monts\OneDrive\Documentos\Escuela\Cinvestav\Primer Cuatrimestre\RFI\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA46FDD9-E678-4790-B81E-1B973E40D7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10524485-5F81-427F-AD52-4CCBB6BCC72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{123A8AA9-D291-44EE-A285-0562C51A2FBD}"/>
+    <workbookView xWindow="-28920" yWindow="-6435" windowWidth="29040" windowHeight="15720" xr2:uid="{123A8AA9-D291-44EE-A285-0562C51A2FBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Nodo inicial</t>
   </si>
@@ -53,43 +53,31 @@
     <t>valor</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>N1</t>
   </si>
   <si>
-    <t>N3</t>
-  </si>
-  <si>
     <t>N2</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>N0</t>
-  </si>
-  <si>
-    <t>SSC</t>
-  </si>
-  <si>
-    <t>SSC1</t>
-  </si>
-  <si>
     <t>longitudElectrica</t>
   </si>
   <si>
     <t>Frecuencia</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>SOC1</t>
+  </si>
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -139,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -152,9 +140,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,7 +457,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,103 +482,71 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>0.61209999999999998</v>
+        <v>13.2629</v>
       </c>
       <c r="F2">
         <v>45</v>
       </c>
       <c r="G2" s="5">
-        <v>1000000</v>
+        <v>1000000000</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1">
-        <v>53</v>
-      </c>
-      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1E-8</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="4">
-        <v>4.6999999999999997E-8</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1">
-        <v>95</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>